<commit_message>
fixed (lkinduh) the times
</commit_message>
<xml_diff>
--- a/base_VS_extension_VS_biased.xlsx
+++ b/base_VS_extension_VS_biased.xlsx
@@ -37,7 +37,7 @@
       <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -60,6 +60,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="00E2EFDA"/>
         <bgColor rgb="00E2EFDA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFF2CC"/>
+        <bgColor rgb="00FFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FCE4D6"/>
+        <bgColor rgb="00FCE4D6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00EDEDED"/>
+        <bgColor rgb="00EDEDED"/>
       </patternFill>
     </fill>
   </fills>
@@ -102,7 +120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -113,6 +131,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,7 +502,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:X22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,6 +525,15 @@
     <col width="13" customWidth="1" min="13" max="13"/>
     <col width="16" customWidth="1" min="14" max="14"/>
     <col width="16" customWidth="1" min="15" max="15"/>
+    <col width="20" customWidth="1" min="16" max="16"/>
+    <col width="24" customWidth="1" min="17" max="17"/>
+    <col width="26" customWidth="1" min="18" max="18"/>
+    <col width="19" customWidth="1" min="19" max="19"/>
+    <col width="23" customWidth="1" min="20" max="20"/>
+    <col width="25" customWidth="1" min="21" max="21"/>
+    <col width="17" customWidth="1" min="22" max="22"/>
+    <col width="21" customWidth="1" min="23" max="23"/>
+    <col width="23" customWidth="1" min="24" max="24"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -579,6 +612,51 @@
           <t>biased_psr_sum</t>
         </is>
       </c>
+      <c r="P1" s="2" t="inlineStr">
+        <is>
+          <t>baseline_prep_time</t>
+        </is>
+      </c>
+      <c r="Q1" s="2" t="inlineStr">
+        <is>
+          <t>gridsampling_prep_time</t>
+        </is>
+      </c>
+      <c r="R1" s="2" t="inlineStr">
+        <is>
+          <t>biasedsampling_prep_time</t>
+        </is>
+      </c>
+      <c r="S1" s="2" t="inlineStr">
+        <is>
+          <t>baseline_sel_time</t>
+        </is>
+      </c>
+      <c r="T1" s="2" t="inlineStr">
+        <is>
+          <t>gridsampling_sel_time</t>
+        </is>
+      </c>
+      <c r="U1" s="2" t="inlineStr">
+        <is>
+          <t>biasedsampling_sel_time</t>
+        </is>
+      </c>
+      <c r="V1" s="2" t="inlineStr">
+        <is>
+          <t>baseline_x_time</t>
+        </is>
+      </c>
+      <c r="W1" s="2" t="inlineStr">
+        <is>
+          <t>gridsampling_x_time</t>
+        </is>
+      </c>
+      <c r="X1" s="2" t="inlineStr">
+        <is>
+          <t>biasedsampling_x_time</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
@@ -611,22 +689,49 @@
         <v>5545.476</v>
       </c>
       <c r="J2" s="5" t="n">
-        <v>0.313</v>
+        <v>0.315</v>
       </c>
       <c r="K2" s="5" t="n">
-        <v>6160.084</v>
+        <v>5855.832</v>
       </c>
       <c r="L2" s="5" t="n">
-        <v>5571.126</v>
+        <v>5052.066</v>
       </c>
       <c r="M2" s="5" t="n">
-        <v>0.343</v>
+        <v>0.427</v>
       </c>
       <c r="N2" s="5" t="n">
-        <v>5657.153</v>
-      </c>
-      <c r="O2" s="5" t="n">
-        <v>4710.319</v>
+        <v>5652.276</v>
+      </c>
+      <c r="O2" s="6" t="n">
+        <v>4624.987</v>
+      </c>
+      <c r="P2" s="7" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="Q2" s="7" t="n">
+        <v>0.00118</v>
+      </c>
+      <c r="R2" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" s="9" t="n">
+        <v>0.00941</v>
+      </c>
+      <c r="T2" s="9" t="n">
+        <v>6e-05</v>
+      </c>
+      <c r="U2" s="10" t="n">
+        <v>4e-05</v>
+      </c>
+      <c r="V2" s="11" t="n">
+        <v>1.719</v>
+      </c>
+      <c r="W2" s="11" t="n">
+        <v>0.00123</v>
+      </c>
+      <c r="X2" s="11" t="n">
+        <v>4e-05</v>
       </c>
     </row>
     <row r="3">
@@ -660,22 +765,49 @@
         <v>5545.476</v>
       </c>
       <c r="J3" s="5" t="n">
-        <v>0.384</v>
+        <v>0.314</v>
       </c>
       <c r="K3" s="5" t="n">
-        <v>5823.186</v>
+        <v>5824.265</v>
       </c>
       <c r="L3" s="5" t="n">
-        <v>4849.528</v>
+        <v>4844.104</v>
       </c>
       <c r="M3" s="5" t="n">
-        <v>0.343</v>
+        <v>0.427</v>
       </c>
       <c r="N3" s="5" t="n">
-        <v>5657.153</v>
-      </c>
-      <c r="O3" s="5" t="n">
-        <v>4710.319</v>
+        <v>5652.276</v>
+      </c>
+      <c r="O3" s="6" t="n">
+        <v>4624.987</v>
+      </c>
+      <c r="P3" s="7" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="Q3" s="7" t="n">
+        <v>0.00125</v>
+      </c>
+      <c r="R3" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" s="9" t="n">
+        <v>0.00941</v>
+      </c>
+      <c r="T3" s="9" t="n">
+        <v>6.999999999999999e-05</v>
+      </c>
+      <c r="U3" s="10" t="n">
+        <v>4e-05</v>
+      </c>
+      <c r="V3" s="11" t="n">
+        <v>1.719</v>
+      </c>
+      <c r="W3" s="11" t="n">
+        <v>0.00131</v>
+      </c>
+      <c r="X3" s="11" t="n">
+        <v>4e-05</v>
       </c>
     </row>
     <row r="4">
@@ -709,22 +841,49 @@
         <v>5545.476</v>
       </c>
       <c r="J4" s="5" t="n">
-        <v>0.321</v>
+        <v>0.395</v>
       </c>
       <c r="K4" s="5" t="n">
-        <v>5997.632</v>
+        <v>6019.135</v>
       </c>
       <c r="L4" s="5" t="n">
-        <v>5255.018</v>
+        <v>5214.014</v>
       </c>
       <c r="M4" s="5" t="n">
-        <v>0.343</v>
+        <v>0.427</v>
       </c>
       <c r="N4" s="5" t="n">
-        <v>5657.153</v>
-      </c>
-      <c r="O4" s="5" t="n">
-        <v>4710.319</v>
+        <v>5652.276</v>
+      </c>
+      <c r="O4" s="6" t="n">
+        <v>4624.987</v>
+      </c>
+      <c r="P4" s="7" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="Q4" s="7" t="n">
+        <v>0.00123</v>
+      </c>
+      <c r="R4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" s="9" t="n">
+        <v>0.00941</v>
+      </c>
+      <c r="T4" s="9" t="n">
+        <v>6e-05</v>
+      </c>
+      <c r="U4" s="10" t="n">
+        <v>4e-05</v>
+      </c>
+      <c r="V4" s="11" t="n">
+        <v>1.719</v>
+      </c>
+      <c r="W4" s="11" t="n">
+        <v>0.00129</v>
+      </c>
+      <c r="X4" s="11" t="n">
+        <v>4e-05</v>
       </c>
     </row>
     <row r="5">
@@ -758,22 +917,49 @@
         <v>11752.429</v>
       </c>
       <c r="J5" s="5" t="n">
-        <v>0.297</v>
+        <v>0.344</v>
       </c>
       <c r="K5" s="5" t="n">
-        <v>11703.198</v>
+        <v>11632.68</v>
       </c>
       <c r="L5" s="5" t="n">
-        <v>10682.969</v>
+        <v>10546.871</v>
       </c>
       <c r="M5" s="5" t="n">
-        <v>0.311</v>
+        <v>0.301</v>
       </c>
       <c r="N5" s="5" t="n">
-        <v>11758.52</v>
-      </c>
-      <c r="O5" s="5" t="n">
-        <v>11533.565</v>
+        <v>12055.906</v>
+      </c>
+      <c r="O5" s="6" t="n">
+        <v>12583.284</v>
+      </c>
+      <c r="P5" s="7" t="n">
+        <v>1.655</v>
+      </c>
+      <c r="Q5" s="7" t="n">
+        <v>0.00119</v>
+      </c>
+      <c r="R5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" s="9" t="n">
+        <v>0.018</v>
+      </c>
+      <c r="T5" s="9" t="n">
+        <v>5e-05</v>
+      </c>
+      <c r="U5" s="10" t="n">
+        <v>3e-05</v>
+      </c>
+      <c r="V5" s="11" t="n">
+        <v>1.673</v>
+      </c>
+      <c r="W5" s="11" t="n">
+        <v>0.00124</v>
+      </c>
+      <c r="X5" s="11" t="n">
+        <v>3e-05</v>
       </c>
     </row>
     <row r="6">
@@ -807,22 +993,49 @@
         <v>11752.429</v>
       </c>
       <c r="J6" s="5" t="n">
-        <v>0.334</v>
+        <v>0.354</v>
       </c>
       <c r="K6" s="5" t="n">
-        <v>11787.873</v>
+        <v>11732.853</v>
       </c>
       <c r="L6" s="5" t="n">
-        <v>10882.99</v>
+        <v>10803.584</v>
       </c>
       <c r="M6" s="5" t="n">
-        <v>0.311</v>
+        <v>0.301</v>
       </c>
       <c r="N6" s="5" t="n">
-        <v>11758.52</v>
-      </c>
-      <c r="O6" s="5" t="n">
-        <v>11533.565</v>
+        <v>12055.906</v>
+      </c>
+      <c r="O6" s="6" t="n">
+        <v>12583.284</v>
+      </c>
+      <c r="P6" s="7" t="n">
+        <v>1.655</v>
+      </c>
+      <c r="Q6" s="7" t="n">
+        <v>0.00123</v>
+      </c>
+      <c r="R6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" s="9" t="n">
+        <v>0.018</v>
+      </c>
+      <c r="T6" s="9" t="n">
+        <v>6.999999999999999e-05</v>
+      </c>
+      <c r="U6" s="10" t="n">
+        <v>3e-05</v>
+      </c>
+      <c r="V6" s="11" t="n">
+        <v>1.673</v>
+      </c>
+      <c r="W6" s="11" t="n">
+        <v>0.0013</v>
+      </c>
+      <c r="X6" s="11" t="n">
+        <v>3e-05</v>
       </c>
     </row>
     <row r="7">
@@ -856,22 +1069,49 @@
         <v>11752.429</v>
       </c>
       <c r="J7" s="5" t="n">
-        <v>0.379</v>
+        <v>0.295</v>
       </c>
       <c r="K7" s="5" t="n">
-        <v>11790.094</v>
+        <v>12111.682</v>
       </c>
       <c r="L7" s="5" t="n">
-        <v>10882.094</v>
+        <v>11529.558</v>
       </c>
       <c r="M7" s="5" t="n">
-        <v>0.311</v>
+        <v>0.301</v>
       </c>
       <c r="N7" s="5" t="n">
-        <v>11758.52</v>
-      </c>
-      <c r="O7" s="5" t="n">
-        <v>11533.565</v>
+        <v>12055.906</v>
+      </c>
+      <c r="O7" s="6" t="n">
+        <v>12583.284</v>
+      </c>
+      <c r="P7" s="7" t="n">
+        <v>1.655</v>
+      </c>
+      <c r="Q7" s="7" t="n">
+        <v>0.00129</v>
+      </c>
+      <c r="R7" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" s="9" t="n">
+        <v>0.018</v>
+      </c>
+      <c r="T7" s="9" t="n">
+        <v>6.999999999999999e-05</v>
+      </c>
+      <c r="U7" s="10" t="n">
+        <v>3e-05</v>
+      </c>
+      <c r="V7" s="11" t="n">
+        <v>1.673</v>
+      </c>
+      <c r="W7" s="11" t="n">
+        <v>0.00136</v>
+      </c>
+      <c r="X7" s="11" t="n">
+        <v>3e-05</v>
       </c>
     </row>
     <row r="8">
@@ -905,22 +1145,49 @@
         <v>30191.783</v>
       </c>
       <c r="J8" s="5" t="n">
-        <v>0.311</v>
+        <v>0.31</v>
       </c>
       <c r="K8" s="5" t="n">
-        <v>29189.54</v>
+        <v>29694.112</v>
       </c>
       <c r="L8" s="5" t="n">
-        <v>27945.276</v>
+        <v>28937.186</v>
       </c>
       <c r="M8" s="5" t="n">
-        <v>0.296</v>
+        <v>0.306</v>
       </c>
       <c r="N8" s="5" t="n">
-        <v>29478.443</v>
-      </c>
-      <c r="O8" s="5" t="n">
-        <v>29056.923</v>
+        <v>28712.173</v>
+      </c>
+      <c r="O8" s="6" t="n">
+        <v>28126.527</v>
+      </c>
+      <c r="P8" s="7" t="n">
+        <v>1.684</v>
+      </c>
+      <c r="Q8" s="7" t="n">
+        <v>0.00121</v>
+      </c>
+      <c r="R8" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" s="9" t="n">
+        <v>0.049</v>
+      </c>
+      <c r="T8" s="9" t="n">
+        <v>6.999999999999999e-05</v>
+      </c>
+      <c r="U8" s="10" t="n">
+        <v>5e-05</v>
+      </c>
+      <c r="V8" s="11" t="n">
+        <v>1.733</v>
+      </c>
+      <c r="W8" s="11" t="n">
+        <v>0.00128</v>
+      </c>
+      <c r="X8" s="11" t="n">
+        <v>5e-05</v>
       </c>
     </row>
     <row r="9">
@@ -957,19 +1224,46 @@
         <v>0.313</v>
       </c>
       <c r="K9" s="5" t="n">
-        <v>29577.114</v>
+        <v>29780.489</v>
       </c>
       <c r="L9" s="5" t="n">
-        <v>28718.377</v>
+        <v>29091.199</v>
       </c>
       <c r="M9" s="5" t="n">
-        <v>0.296</v>
+        <v>0.306</v>
       </c>
       <c r="N9" s="5" t="n">
-        <v>29478.443</v>
-      </c>
-      <c r="O9" s="5" t="n">
-        <v>29056.923</v>
+        <v>28712.173</v>
+      </c>
+      <c r="O9" s="6" t="n">
+        <v>28126.527</v>
+      </c>
+      <c r="P9" s="7" t="n">
+        <v>1.684</v>
+      </c>
+      <c r="Q9" s="7" t="n">
+        <v>0.00122</v>
+      </c>
+      <c r="R9" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" s="9" t="n">
+        <v>0.049</v>
+      </c>
+      <c r="T9" s="9" t="n">
+        <v>8.000000000000001e-05</v>
+      </c>
+      <c r="U9" s="10" t="n">
+        <v>5e-05</v>
+      </c>
+      <c r="V9" s="11" t="n">
+        <v>1.733</v>
+      </c>
+      <c r="W9" s="11" t="n">
+        <v>0.0013</v>
+      </c>
+      <c r="X9" s="11" t="n">
+        <v>5e-05</v>
       </c>
     </row>
     <row r="10">
@@ -1003,22 +1297,49 @@
         <v>30191.783</v>
       </c>
       <c r="J10" s="5" t="n">
-        <v>0.326</v>
+        <v>0.321</v>
       </c>
       <c r="K10" s="5" t="n">
-        <v>29893.996</v>
+        <v>29633.916</v>
       </c>
       <c r="L10" s="5" t="n">
-        <v>29318.512</v>
+        <v>28781.372</v>
       </c>
       <c r="M10" s="5" t="n">
-        <v>0.296</v>
+        <v>0.306</v>
       </c>
       <c r="N10" s="5" t="n">
-        <v>29478.443</v>
-      </c>
-      <c r="O10" s="5" t="n">
-        <v>29056.923</v>
+        <v>28712.173</v>
+      </c>
+      <c r="O10" s="6" t="n">
+        <v>28126.527</v>
+      </c>
+      <c r="P10" s="7" t="n">
+        <v>1.684</v>
+      </c>
+      <c r="Q10" s="7" t="n">
+        <v>0.00122</v>
+      </c>
+      <c r="R10" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" s="9" t="n">
+        <v>0.049</v>
+      </c>
+      <c r="T10" s="9" t="n">
+        <v>9.000000000000001e-05</v>
+      </c>
+      <c r="U10" s="10" t="n">
+        <v>5e-05</v>
+      </c>
+      <c r="V10" s="11" t="n">
+        <v>1.733</v>
+      </c>
+      <c r="W10" s="11" t="n">
+        <v>0.00131</v>
+      </c>
+      <c r="X10" s="11" t="n">
+        <v>5e-05</v>
       </c>
     </row>
     <row r="11">
@@ -1052,22 +1373,49 @@
         <v>61150.778</v>
       </c>
       <c r="J11" s="5" t="n">
+        <v>0.302</v>
+      </c>
+      <c r="K11" s="5" t="n">
+        <v>59168.182</v>
+      </c>
+      <c r="L11" s="5" t="n">
+        <v>58349.513</v>
+      </c>
+      <c r="M11" s="5" t="n">
         <v>0.306</v>
       </c>
-      <c r="K11" s="5" t="n">
-        <v>59048.874</v>
-      </c>
-      <c r="L11" s="5" t="n">
-        <v>58158.585</v>
-      </c>
-      <c r="M11" s="5" t="n">
-        <v>0.308</v>
-      </c>
       <c r="N11" s="5" t="n">
-        <v>58946.965</v>
-      </c>
-      <c r="O11" s="5" t="n">
-        <v>58011.666</v>
+        <v>58504.923</v>
+      </c>
+      <c r="O11" s="6" t="n">
+        <v>57216.278</v>
+      </c>
+      <c r="P11" s="7" t="n">
+        <v>1.663</v>
+      </c>
+      <c r="Q11" s="7" t="n">
+        <v>0.00126</v>
+      </c>
+      <c r="R11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" s="9" t="n">
+        <v>0.091</v>
+      </c>
+      <c r="T11" s="9" t="n">
+        <v>9.000000000000001e-05</v>
+      </c>
+      <c r="U11" s="10" t="n">
+        <v>6e-05</v>
+      </c>
+      <c r="V11" s="11" t="n">
+        <v>1.754</v>
+      </c>
+      <c r="W11" s="11" t="n">
+        <v>0.00135</v>
+      </c>
+      <c r="X11" s="11" t="n">
+        <v>6e-05</v>
       </c>
     </row>
     <row r="12">
@@ -1101,22 +1449,49 @@
         <v>61150.778</v>
       </c>
       <c r="J12" s="5" t="n">
-        <v>0.305</v>
+        <v>0.313</v>
       </c>
       <c r="K12" s="5" t="n">
-        <v>59132.96</v>
+        <v>58994.246</v>
       </c>
       <c r="L12" s="5" t="n">
-        <v>58252.138</v>
+        <v>57999.373</v>
       </c>
       <c r="M12" s="5" t="n">
-        <v>0.308</v>
+        <v>0.306</v>
       </c>
       <c r="N12" s="5" t="n">
-        <v>58946.965</v>
-      </c>
-      <c r="O12" s="5" t="n">
-        <v>58011.666</v>
+        <v>58504.923</v>
+      </c>
+      <c r="O12" s="6" t="n">
+        <v>57216.278</v>
+      </c>
+      <c r="P12" s="7" t="n">
+        <v>1.663</v>
+      </c>
+      <c r="Q12" s="7" t="n">
+        <v>0.00123</v>
+      </c>
+      <c r="R12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" s="9" t="n">
+        <v>0.091</v>
+      </c>
+      <c r="T12" s="9" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="U12" s="10" t="n">
+        <v>6e-05</v>
+      </c>
+      <c r="V12" s="11" t="n">
+        <v>1.754</v>
+      </c>
+      <c r="W12" s="11" t="n">
+        <v>0.00133</v>
+      </c>
+      <c r="X12" s="11" t="n">
+        <v>6e-05</v>
       </c>
     </row>
     <row r="13">
@@ -1150,22 +1525,49 @@
         <v>61150.778</v>
       </c>
       <c r="J13" s="5" t="n">
-        <v>0.292</v>
+        <v>0.306</v>
       </c>
       <c r="K13" s="5" t="n">
-        <v>59378.126</v>
+        <v>59791.284</v>
       </c>
       <c r="L13" s="5" t="n">
-        <v>58740.46</v>
+        <v>59615.576</v>
       </c>
       <c r="M13" s="5" t="n">
-        <v>0.308</v>
+        <v>0.306</v>
       </c>
       <c r="N13" s="5" t="n">
-        <v>58946.965</v>
-      </c>
-      <c r="O13" s="5" t="n">
-        <v>58011.666</v>
+        <v>58504.923</v>
+      </c>
+      <c r="O13" s="6" t="n">
+        <v>57216.278</v>
+      </c>
+      <c r="P13" s="7" t="n">
+        <v>1.663</v>
+      </c>
+      <c r="Q13" s="7" t="n">
+        <v>0.0012</v>
+      </c>
+      <c r="R13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" s="9" t="n">
+        <v>0.091</v>
+      </c>
+      <c r="T13" s="9" t="n">
+        <v>0.00014</v>
+      </c>
+      <c r="U13" s="10" t="n">
+        <v>6e-05</v>
+      </c>
+      <c r="V13" s="11" t="n">
+        <v>1.754</v>
+      </c>
+      <c r="W13" s="11" t="n">
+        <v>0.00134</v>
+      </c>
+      <c r="X13" s="11" t="n">
+        <v>6e-05</v>
       </c>
     </row>
     <row r="14">
@@ -1199,22 +1601,49 @@
         <v>56212.719</v>
       </c>
       <c r="J14" s="5" t="n">
-        <v>0.338</v>
+        <v>0.281</v>
       </c>
       <c r="K14" s="5" t="n">
-        <v>56303.156</v>
+        <v>58687.897</v>
       </c>
       <c r="L14" s="5" t="n">
-        <v>51065.596</v>
+        <v>56680.279</v>
       </c>
       <c r="M14" s="5" t="n">
-        <v>0.317</v>
+        <v>0.298</v>
       </c>
       <c r="N14" s="5" t="n">
-        <v>55521.85</v>
-      </c>
-      <c r="O14" s="5" t="n">
-        <v>50384.289</v>
+        <v>58285.414</v>
+      </c>
+      <c r="O14" s="6" t="n">
+        <v>55794.352</v>
+      </c>
+      <c r="P14" s="7" t="n">
+        <v>41.376</v>
+      </c>
+      <c r="Q14" s="7" t="n">
+        <v>0.00643</v>
+      </c>
+      <c r="R14" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" s="9" t="n">
+        <v>0.106</v>
+      </c>
+      <c r="T14" s="9" t="n">
+        <v>6.999999999999999e-05</v>
+      </c>
+      <c r="U14" s="10" t="n">
+        <v>3e-05</v>
+      </c>
+      <c r="V14" s="11" t="n">
+        <v>41.483</v>
+      </c>
+      <c r="W14" s="11" t="n">
+        <v>0.0065</v>
+      </c>
+      <c r="X14" s="11" t="n">
+        <v>3e-05</v>
       </c>
     </row>
     <row r="15">
@@ -1248,22 +1677,49 @@
         <v>56212.719</v>
       </c>
       <c r="J15" s="5" t="n">
-        <v>0.316</v>
+        <v>0.319</v>
       </c>
       <c r="K15" s="5" t="n">
-        <v>55625.195</v>
+        <v>56086.64</v>
       </c>
       <c r="L15" s="5" t="n">
-        <v>49693.528</v>
+        <v>50629.385</v>
       </c>
       <c r="M15" s="5" t="n">
-        <v>0.317</v>
+        <v>0.298</v>
       </c>
       <c r="N15" s="5" t="n">
-        <v>55521.85</v>
-      </c>
-      <c r="O15" s="5" t="n">
-        <v>50384.289</v>
+        <v>58285.414</v>
+      </c>
+      <c r="O15" s="6" t="n">
+        <v>55794.352</v>
+      </c>
+      <c r="P15" s="7" t="n">
+        <v>41.376</v>
+      </c>
+      <c r="Q15" s="7" t="n">
+        <v>0.00594</v>
+      </c>
+      <c r="R15" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" s="9" t="n">
+        <v>0.106</v>
+      </c>
+      <c r="T15" s="9" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="U15" s="10" t="n">
+        <v>3e-05</v>
+      </c>
+      <c r="V15" s="11" t="n">
+        <v>41.483</v>
+      </c>
+      <c r="W15" s="11" t="n">
+        <v>0.00604</v>
+      </c>
+      <c r="X15" s="11" t="n">
+        <v>3e-05</v>
       </c>
     </row>
     <row r="16">
@@ -1297,22 +1753,49 @@
         <v>56212.719</v>
       </c>
       <c r="J16" s="5" t="n">
-        <v>0.319</v>
+        <v>0.341</v>
       </c>
       <c r="K16" s="5" t="n">
-        <v>56048.898</v>
+        <v>57536.715</v>
       </c>
       <c r="L16" s="5" t="n">
-        <v>50500.238</v>
+        <v>53566.773</v>
       </c>
       <c r="M16" s="5" t="n">
-        <v>0.317</v>
+        <v>0.298</v>
       </c>
       <c r="N16" s="5" t="n">
-        <v>55521.85</v>
-      </c>
-      <c r="O16" s="5" t="n">
-        <v>50384.289</v>
+        <v>58285.414</v>
+      </c>
+      <c r="O16" s="6" t="n">
+        <v>55794.352</v>
+      </c>
+      <c r="P16" s="7" t="n">
+        <v>41.376</v>
+      </c>
+      <c r="Q16" s="7" t="n">
+        <v>0.00646</v>
+      </c>
+      <c r="R16" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" s="9" t="n">
+        <v>0.106</v>
+      </c>
+      <c r="T16" s="9" t="n">
+        <v>8.000000000000001e-05</v>
+      </c>
+      <c r="U16" s="10" t="n">
+        <v>3e-05</v>
+      </c>
+      <c r="V16" s="11" t="n">
+        <v>41.483</v>
+      </c>
+      <c r="W16" s="11" t="n">
+        <v>0.00654</v>
+      </c>
+      <c r="X16" s="11" t="n">
+        <v>3e-05</v>
       </c>
     </row>
     <row r="17">
@@ -1346,22 +1829,49 @@
         <v>146377.806</v>
       </c>
       <c r="J17" s="5" t="n">
-        <v>0.311</v>
+        <v>0.303</v>
       </c>
       <c r="K17" s="5" t="n">
-        <v>142156.663</v>
+        <v>144172.804</v>
       </c>
       <c r="L17" s="5" t="n">
-        <v>137777.349</v>
+        <v>141656.809</v>
       </c>
       <c r="M17" s="5" t="n">
-        <v>0.31</v>
+        <v>0.317</v>
       </c>
       <c r="N17" s="5" t="n">
-        <v>143834.695</v>
-      </c>
-      <c r="O17" s="5" t="n">
-        <v>141823.991</v>
+        <v>141177.096</v>
+      </c>
+      <c r="O17" s="6" t="n">
+        <v>135870.034</v>
+      </c>
+      <c r="P17" s="7" t="n">
+        <v>40.918</v>
+      </c>
+      <c r="Q17" s="7" t="n">
+        <v>0.00644</v>
+      </c>
+      <c r="R17" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" s="9" t="n">
+        <v>0.267</v>
+      </c>
+      <c r="T17" s="9" t="n">
+        <v>6.999999999999999e-05</v>
+      </c>
+      <c r="U17" s="10" t="n">
+        <v>6e-05</v>
+      </c>
+      <c r="V17" s="11" t="n">
+        <v>41.185</v>
+      </c>
+      <c r="W17" s="11" t="n">
+        <v>0.00651</v>
+      </c>
+      <c r="X17" s="11" t="n">
+        <v>6e-05</v>
       </c>
     </row>
     <row r="18">
@@ -1395,22 +1905,49 @@
         <v>146377.806</v>
       </c>
       <c r="J18" s="5" t="n">
-        <v>0.296</v>
+        <v>0.309</v>
       </c>
       <c r="K18" s="5" t="n">
-        <v>145259.056</v>
+        <v>143595.144</v>
       </c>
       <c r="L18" s="5" t="n">
-        <v>143523.652</v>
+        <v>140099.27</v>
       </c>
       <c r="M18" s="5" t="n">
-        <v>0.31</v>
+        <v>0.317</v>
       </c>
       <c r="N18" s="5" t="n">
-        <v>143834.695</v>
-      </c>
-      <c r="O18" s="5" t="n">
-        <v>141823.991</v>
+        <v>141177.096</v>
+      </c>
+      <c r="O18" s="6" t="n">
+        <v>135870.034</v>
+      </c>
+      <c r="P18" s="7" t="n">
+        <v>40.918</v>
+      </c>
+      <c r="Q18" s="7" t="n">
+        <v>0.00597</v>
+      </c>
+      <c r="R18" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" s="9" t="n">
+        <v>0.267</v>
+      </c>
+      <c r="T18" s="9" t="n">
+        <v>8.000000000000001e-05</v>
+      </c>
+      <c r="U18" s="10" t="n">
+        <v>6e-05</v>
+      </c>
+      <c r="V18" s="11" t="n">
+        <v>41.185</v>
+      </c>
+      <c r="W18" s="11" t="n">
+        <v>0.00605</v>
+      </c>
+      <c r="X18" s="11" t="n">
+        <v>6e-05</v>
       </c>
     </row>
     <row r="19">
@@ -1444,22 +1981,49 @@
         <v>146377.806</v>
       </c>
       <c r="J19" s="5" t="n">
-        <v>0.309</v>
+        <v>0.326</v>
       </c>
       <c r="K19" s="5" t="n">
-        <v>142528.392</v>
+        <v>142081.747</v>
       </c>
       <c r="L19" s="5" t="n">
-        <v>137880.999</v>
+        <v>137031.914</v>
       </c>
       <c r="M19" s="5" t="n">
-        <v>0.31</v>
+        <v>0.317</v>
       </c>
       <c r="N19" s="5" t="n">
-        <v>143834.695</v>
-      </c>
-      <c r="O19" s="5" t="n">
-        <v>141823.991</v>
+        <v>141177.096</v>
+      </c>
+      <c r="O19" s="6" t="n">
+        <v>135870.034</v>
+      </c>
+      <c r="P19" s="7" t="n">
+        <v>40.918</v>
+      </c>
+      <c r="Q19" s="7" t="n">
+        <v>0.00615</v>
+      </c>
+      <c r="R19" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" s="9" t="n">
+        <v>0.267</v>
+      </c>
+      <c r="T19" s="9" t="n">
+        <v>9.000000000000001e-05</v>
+      </c>
+      <c r="U19" s="10" t="n">
+        <v>6e-05</v>
+      </c>
+      <c r="V19" s="11" t="n">
+        <v>41.185</v>
+      </c>
+      <c r="W19" s="11" t="n">
+        <v>0.00624</v>
+      </c>
+      <c r="X19" s="11" t="n">
+        <v>6e-05</v>
       </c>
     </row>
     <row r="20">
@@ -1493,22 +2057,49 @@
         <v>295377.945</v>
       </c>
       <c r="J20" s="5" t="n">
-        <v>0.307</v>
+        <v>0.305</v>
       </c>
       <c r="K20" s="5" t="n">
-        <v>283647.707</v>
+        <v>286784.764</v>
       </c>
       <c r="L20" s="5" t="n">
-        <v>278138.103</v>
+        <v>284131.814</v>
       </c>
       <c r="M20" s="5" t="n">
-        <v>0.3</v>
+        <v>0.309</v>
       </c>
       <c r="N20" s="5" t="n">
-        <v>283785.177</v>
-      </c>
-      <c r="O20" s="5" t="n">
-        <v>278292.253</v>
+        <v>284164.858</v>
+      </c>
+      <c r="O20" s="6" t="n">
+        <v>282440.001</v>
+      </c>
+      <c r="P20" s="7" t="n">
+        <v>41.272</v>
+      </c>
+      <c r="Q20" s="7" t="n">
+        <v>0.00643</v>
+      </c>
+      <c r="R20" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S20" s="9" t="n">
+        <v>0.539</v>
+      </c>
+      <c r="T20" s="9" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="U20" s="10" t="n">
+        <v>6.999999999999999e-05</v>
+      </c>
+      <c r="V20" s="11" t="n">
+        <v>41.812</v>
+      </c>
+      <c r="W20" s="11" t="n">
+        <v>0.00653</v>
+      </c>
+      <c r="X20" s="11" t="n">
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="21">
@@ -1542,22 +2133,49 @@
         <v>295377.945</v>
       </c>
       <c r="J21" s="5" t="n">
-        <v>0.31</v>
+        <v>0.291</v>
       </c>
       <c r="K21" s="5" t="n">
-        <v>285762.577</v>
+        <v>284131.583</v>
       </c>
       <c r="L21" s="5" t="n">
-        <v>281926.735</v>
+        <v>278510.333</v>
       </c>
       <c r="M21" s="5" t="n">
-        <v>0.3</v>
+        <v>0.309</v>
       </c>
       <c r="N21" s="5" t="n">
-        <v>283785.177</v>
-      </c>
-      <c r="O21" s="5" t="n">
-        <v>278292.253</v>
+        <v>284164.858</v>
+      </c>
+      <c r="O21" s="6" t="n">
+        <v>282440.001</v>
+      </c>
+      <c r="P21" s="7" t="n">
+        <v>41.272</v>
+      </c>
+      <c r="Q21" s="7" t="n">
+        <v>0.00609</v>
+      </c>
+      <c r="R21" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S21" s="9" t="n">
+        <v>0.539</v>
+      </c>
+      <c r="T21" s="9" t="n">
+        <v>0.00012</v>
+      </c>
+      <c r="U21" s="10" t="n">
+        <v>6.999999999999999e-05</v>
+      </c>
+      <c r="V21" s="11" t="n">
+        <v>41.812</v>
+      </c>
+      <c r="W21" s="11" t="n">
+        <v>0.00621</v>
+      </c>
+      <c r="X21" s="11" t="n">
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="22">
@@ -1591,22 +2209,49 @@
         <v>295377.945</v>
       </c>
       <c r="J22" s="5" t="n">
-        <v>0.296</v>
+        <v>0.311</v>
       </c>
       <c r="K22" s="5" t="n">
-        <v>285355.818</v>
+        <v>283436.917</v>
       </c>
       <c r="L22" s="5" t="n">
-        <v>280908.64</v>
+        <v>277206.708</v>
       </c>
       <c r="M22" s="5" t="n">
-        <v>0.3</v>
+        <v>0.309</v>
       </c>
       <c r="N22" s="5" t="n">
-        <v>283785.177</v>
-      </c>
-      <c r="O22" s="5" t="n">
-        <v>278292.253</v>
+        <v>284164.858</v>
+      </c>
+      <c r="O22" s="6" t="n">
+        <v>282440.001</v>
+      </c>
+      <c r="P22" s="7" t="n">
+        <v>41.272</v>
+      </c>
+      <c r="Q22" s="7" t="n">
+        <v>0.00647</v>
+      </c>
+      <c r="R22" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S22" s="9" t="n">
+        <v>0.539</v>
+      </c>
+      <c r="T22" s="9" t="n">
+        <v>0.00012</v>
+      </c>
+      <c r="U22" s="10" t="n">
+        <v>6.999999999999999e-05</v>
+      </c>
+      <c r="V22" s="11" t="n">
+        <v>41.812</v>
+      </c>
+      <c r="W22" s="11" t="n">
+        <v>0.00659</v>
+      </c>
+      <c r="X22" s="11" t="n">
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>